<commit_message>
Last version of tables
I forgot to commit the new tables with the offset to make the temperature a natural value...
</commit_message>
<xml_diff>
--- a/Documentation/Fuzzy/Fuzzy Table.xlsx
+++ b/Documentation/Fuzzy/Fuzzy Table.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="51">
   <si>
     <t>2 Entradas:</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Temperatura</t>
   </si>
   <si>
-    <t>El sensor va desde -40 a 130 grados</t>
-  </si>
-  <si>
     <t>Punto1</t>
   </si>
   <si>
@@ -140,21 +137,6 @@
     <t>Points extracted from the software:</t>
   </si>
   <si>
-    <t>8e</t>
-  </si>
-  <si>
-    <t>AC</t>
-  </si>
-  <si>
-    <t>ac</t>
-  </si>
-  <si>
-    <t>bb</t>
-  </si>
-  <si>
-    <t>ca</t>
-  </si>
-  <si>
     <t>ff</t>
   </si>
   <si>
@@ -164,7 +146,28 @@
     <t>bf</t>
   </si>
   <si>
-    <t>pero es feo numero, asi que lo offseteo con +50</t>
+    <t>El sensor va desde -40 a 130 grados pero es feo numero</t>
+  </si>
+  <si>
+    <t>asi que lo offseteo con +50 para fuzzy</t>
+  </si>
+  <si>
+    <t>0D</t>
+  </si>
+  <si>
+    <t>8C</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>F1</t>
   </si>
 </sst>
 </file>
@@ -478,16 +481,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-40</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-40</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -560,16 +563,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>65</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -642,16 +645,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>55</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>75</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>85</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -724,16 +727,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>75</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>85</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>85</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>95</c:v>
+                  <c:v>145</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -806,16 +809,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>85</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>95</c:v>
+                  <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>95</c:v>
+                  <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>105</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -888,16 +891,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>95</c:v>
+                  <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>105</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>130</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>130</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -940,7 +943,7 @@
         <c:axId val="294552624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="-50"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1877,16 +1880,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-40</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-40</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1951,16 +1954,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>65</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2033,16 +2036,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>55</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>75</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>85</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2115,16 +2118,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>75</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>85</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>85</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>95</c:v>
+                  <c:v>145</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2197,16 +2200,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>85</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>95</c:v>
+                  <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>95</c:v>
+                  <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>105</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2279,16 +2282,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>95</c:v>
+                  <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>105</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>130</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>130</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4555,8 +4558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4657,7 +4660,7 @@
     </row>
     <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4805,26 +4808,26 @@
         <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" t="s">
         <v>29</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>30</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>31</v>
-      </c>
-      <c r="E20" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -4846,16 +4849,16 @@
         <v>8</v>
       </c>
       <c r="B22">
-        <v>-40</v>
+        <v>10</v>
       </c>
       <c r="C22">
-        <v>-40</v>
+        <v>10</v>
       </c>
       <c r="D22">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="E22">
-        <v>45</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -4863,16 +4866,16 @@
         <v>9</v>
       </c>
       <c r="B23">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="C23">
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="D23">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="E23">
-        <v>65</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -4880,16 +4883,16 @@
         <v>10</v>
       </c>
       <c r="B24">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="C24">
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="D24">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="E24">
-        <v>85</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -4897,16 +4900,16 @@
         <v>11</v>
       </c>
       <c r="B25">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="C25">
-        <v>85</v>
+        <v>135</v>
       </c>
       <c r="D25">
-        <v>85</v>
+        <v>135</v>
       </c>
       <c r="E25">
-        <v>95</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -4914,16 +4917,16 @@
         <v>12</v>
       </c>
       <c r="B26">
-        <v>85</v>
+        <v>135</v>
       </c>
       <c r="C26">
-        <v>95</v>
+        <v>145</v>
       </c>
       <c r="D26">
-        <v>95</v>
+        <v>145</v>
       </c>
       <c r="E26">
-        <v>105</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -4931,38 +4934,38 @@
         <v>13</v>
       </c>
       <c r="B27">
-        <v>95</v>
+        <v>145</v>
       </c>
       <c r="C27">
-        <v>105</v>
+        <v>155</v>
       </c>
       <c r="D27">
-        <v>130</v>
+        <v>180</v>
       </c>
       <c r="E27">
-        <v>130</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
         <v>33</v>
-      </c>
-      <c r="B29" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" t="s">
         <v>29</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>30</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>31</v>
-      </c>
-      <c r="E31" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -5052,13 +5055,13 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
         <v>38</v>
       </c>
-      <c r="B38" t="s">
+      <c r="G38" t="s">
         <v>39</v>
-      </c>
-      <c r="G38" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
@@ -5066,32 +5069,32 @@
         <v>8</v>
       </c>
       <c r="B40" t="str">
-        <f>DEC2HEX( 60+(255*B22/170))</f>
-        <v>0</v>
+        <f>DEC2HEX( (255*B22/190))</f>
+        <v>D</v>
       </c>
       <c r="C40" t="str">
-        <f t="shared" ref="C40:E40" si="0">DEC2HEX( 60+(255*C22/170))</f>
-        <v>0</v>
+        <f t="shared" ref="C40:E40" si="0">DEC2HEX( (255*C22/190))</f>
+        <v>D</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" si="0"/>
         <v>7F</v>
       </c>
-      <c r="G40">
-        <v>0</v>
+      <c r="G40" t="s">
+        <v>45</v>
       </c>
       <c r="H40">
         <v>0</v>
       </c>
       <c r="I40">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J40">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
@@ -5099,8 +5102,8 @@
         <v>9</v>
       </c>
       <c r="B41" t="str">
-        <f t="shared" ref="B41:E41" si="1">DEC2HEX( 60+(255*B23/170))</f>
-        <v>70</v>
+        <f t="shared" ref="B41:E45" si="1">DEC2HEX( (255*B23/190))</f>
+        <v>72</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="1"/>
@@ -5108,23 +5111,23 @@
       </c>
       <c r="D41" t="str">
         <f t="shared" si="1"/>
-        <v>8E</v>
+        <v>8C</v>
       </c>
       <c r="E41" t="str">
         <f t="shared" si="1"/>
-        <v>9D</v>
+        <v>9A</v>
       </c>
       <c r="G41">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H41">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="I41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="J41">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
@@ -5132,32 +5135,32 @@
         <v>10</v>
       </c>
       <c r="B42" t="str">
-        <f t="shared" ref="B42:E42" si="2">DEC2HEX( 60+(255*B24/170))</f>
-        <v>8E</v>
+        <f t="shared" si="1"/>
+        <v>8C</v>
       </c>
       <c r="C42" t="str">
-        <f t="shared" si="2"/>
-        <v>9D</v>
+        <f t="shared" si="1"/>
+        <v>9A</v>
       </c>
       <c r="D42" t="str">
-        <f t="shared" si="2"/>
-        <v>AC</v>
+        <f t="shared" si="1"/>
+        <v>A7</v>
       </c>
       <c r="E42" t="str">
-        <f t="shared" si="2"/>
-        <v>BB</v>
+        <f t="shared" si="1"/>
+        <v>B5</v>
       </c>
       <c r="G42" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="H42">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I42" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="J42">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
@@ -5165,32 +5168,32 @@
         <v>11</v>
       </c>
       <c r="B43" t="str">
-        <f t="shared" ref="B43:E43" si="3">DEC2HEX( 60+(255*B25/170))</f>
-        <v>AC</v>
+        <f t="shared" si="1"/>
+        <v>A7</v>
       </c>
       <c r="C43" t="str">
-        <f t="shared" si="3"/>
-        <v>BB</v>
+        <f t="shared" si="1"/>
+        <v>B5</v>
       </c>
       <c r="D43" t="str">
-        <f t="shared" si="3"/>
-        <v>BB</v>
+        <f t="shared" si="1"/>
+        <v>B5</v>
       </c>
       <c r="E43" t="str">
-        <f t="shared" si="3"/>
-        <v>CA</v>
+        <f t="shared" si="1"/>
+        <v>C2</v>
       </c>
       <c r="G43" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H43">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I43" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="J43">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
@@ -5198,32 +5201,32 @@
         <v>12</v>
       </c>
       <c r="B44" t="str">
-        <f t="shared" ref="B44:E44" si="4">DEC2HEX( 60+(255*B26/170))</f>
-        <v>BB</v>
+        <f t="shared" si="1"/>
+        <v>B5</v>
       </c>
       <c r="C44" t="str">
-        <f t="shared" si="4"/>
-        <v>CA</v>
+        <f t="shared" si="1"/>
+        <v>C2</v>
       </c>
       <c r="D44" t="str">
-        <f t="shared" si="4"/>
-        <v>CA</v>
+        <f t="shared" si="1"/>
+        <v>C2</v>
       </c>
       <c r="E44" t="str">
-        <f t="shared" si="4"/>
-        <v>D9</v>
+        <f t="shared" si="1"/>
+        <v>D0</v>
       </c>
       <c r="G44" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H44">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="I44" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="J44">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
@@ -5231,29 +5234,29 @@
         <v>13</v>
       </c>
       <c r="B45" t="str">
-        <f t="shared" ref="B45:E45" si="5">DEC2HEX( 60+(255*B27/170))</f>
-        <v>CA</v>
+        <f t="shared" si="1"/>
+        <v>C2</v>
       </c>
       <c r="C45" t="str">
-        <f t="shared" si="5"/>
-        <v>D9</v>
+        <f t="shared" si="1"/>
+        <v>D0</v>
       </c>
       <c r="D45" t="str">
-        <f t="shared" si="5"/>
-        <v>FF</v>
+        <f t="shared" si="1"/>
+        <v>F1</v>
       </c>
       <c r="E45" t="str">
-        <f t="shared" si="5"/>
-        <v>FF</v>
+        <f t="shared" si="1"/>
+        <v>F1</v>
       </c>
       <c r="G45" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="H45">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I45" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="J45">
         <v>0</v>
@@ -5268,15 +5271,15 @@
         <v>0</v>
       </c>
       <c r="C47" t="str">
-        <f t="shared" ref="C47:E47" si="6">DEC2HEX( (255*C32/100))</f>
+        <f t="shared" ref="C47:E47" si="2">DEC2HEX( (255*C32/100))</f>
         <v>0</v>
       </c>
       <c r="D47" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E47" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="G47">
@@ -5289,7 +5292,7 @@
         <v>0</v>
       </c>
       <c r="J47" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
@@ -5297,19 +5300,19 @@
         <v>15</v>
       </c>
       <c r="B48" t="str">
-        <f t="shared" ref="B48:E48" si="7">DEC2HEX( (255*B33/100))</f>
+        <f t="shared" ref="B48:E48" si="3">DEC2HEX( (255*B33/100))</f>
         <v>0</v>
       </c>
       <c r="C48" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>C</v>
       </c>
       <c r="D48" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="E48" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="G48">
@@ -5330,32 +5333,32 @@
         <v>16</v>
       </c>
       <c r="B49" t="str">
-        <f t="shared" ref="B49:E49" si="8">DEC2HEX( (255*B34/100))</f>
+        <f t="shared" ref="B49:E49" si="4">DEC2HEX( (255*B34/100))</f>
         <v>19</v>
       </c>
       <c r="C49" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>33</v>
       </c>
       <c r="D49" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>72</v>
       </c>
       <c r="E49" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>8C</v>
       </c>
       <c r="G49">
         <v>19</v>
       </c>
       <c r="H49" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="I49">
         <v>72</v>
       </c>
       <c r="J49" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
@@ -5363,32 +5366,32 @@
         <v>17</v>
       </c>
       <c r="B50" t="str">
-        <f t="shared" ref="B50:E50" si="9">DEC2HEX( (255*B35/100))</f>
+        <f t="shared" ref="B50:E50" si="5">DEC2HEX( (255*B35/100))</f>
         <v>72</v>
       </c>
       <c r="C50" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>8C</v>
       </c>
       <c r="D50" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>BF</v>
       </c>
       <c r="E50" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>D8</v>
       </c>
       <c r="G50">
         <v>72</v>
       </c>
       <c r="H50" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="I50" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="J50" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
@@ -5396,29 +5399,29 @@
         <v>18</v>
       </c>
       <c r="B51" t="str">
-        <f t="shared" ref="B51:E51" si="10">DEC2HEX( (255*B36/100))</f>
+        <f t="shared" ref="B51:E51" si="6">DEC2HEX( (255*B36/100))</f>
         <v>BF</v>
       </c>
       <c r="C51" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>D8</v>
       </c>
       <c r="D51" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>FF</v>
       </c>
       <c r="E51" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>FF</v>
       </c>
       <c r="G51" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H51" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="I51" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="J51">
         <v>0</v>
@@ -5449,16 +5452,16 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
         <v>35</v>
-      </c>
-      <c r="C3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4">
         <f>Principal!$B$22</f>
-        <v>-40</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -5467,7 +5470,7 @@
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5">
         <f>Principal!$C$22</f>
-        <v>-40</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -5476,7 +5479,7 @@
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6">
         <f>Principal!$D$22</f>
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -5485,7 +5488,7 @@
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7">
         <f>Principal!$E$22</f>
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -5496,16 +5499,16 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
         <v>35</v>
-      </c>
-      <c r="C9" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10">
         <f>Principal!$B$23</f>
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -5514,7 +5517,7 @@
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11">
         <f>Principal!$C$23</f>
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -5523,7 +5526,7 @@
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12">
         <f>Principal!$D$23</f>
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -5532,7 +5535,7 @@
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13">
         <f>Principal!$E$23</f>
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -5543,16 +5546,16 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
         <v>35</v>
-      </c>
-      <c r="C15" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16">
         <f>Principal!$B$24</f>
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -5561,7 +5564,7 @@
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B17">
         <f>Principal!$C$24</f>
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -5570,7 +5573,7 @@
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B18">
         <f>Principal!$D$24</f>
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -5579,7 +5582,7 @@
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19">
         <f>Principal!$E$24</f>
-        <v>85</v>
+        <v>135</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -5590,16 +5593,16 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
         <v>35</v>
-      </c>
-      <c r="C21" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B22">
         <f>Principal!$B$25</f>
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -5608,7 +5611,7 @@
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B23">
         <f>Principal!$C$25</f>
-        <v>85</v>
+        <v>135</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -5617,7 +5620,7 @@
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B24">
         <f>Principal!$D$25</f>
-        <v>85</v>
+        <v>135</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -5626,7 +5629,7 @@
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B25">
         <f>Principal!$E$25</f>
-        <v>95</v>
+        <v>145</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -5637,16 +5640,16 @@
         <v>12</v>
       </c>
       <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
         <v>35</v>
-      </c>
-      <c r="C27" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B28">
         <f>Principal!$B$26</f>
-        <v>85</v>
+        <v>135</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -5655,7 +5658,7 @@
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B29">
         <f>Principal!$C$26</f>
-        <v>95</v>
+        <v>145</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -5664,7 +5667,7 @@
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B30">
         <f>Principal!$D$26</f>
-        <v>95</v>
+        <v>145</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -5673,7 +5676,7 @@
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B31">
         <f>Principal!$E$26</f>
-        <v>105</v>
+        <v>155</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -5684,16 +5687,16 @@
         <v>13</v>
       </c>
       <c r="B33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" t="s">
         <v>35</v>
-      </c>
-      <c r="C33" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B34">
         <f>Principal!$B$27</f>
-        <v>95</v>
+        <v>145</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -5702,7 +5705,7 @@
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B35">
         <f>Principal!$C$27</f>
-        <v>105</v>
+        <v>155</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -5711,7 +5714,7 @@
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B36">
         <f>Principal!$D$27</f>
-        <v>130</v>
+        <v>180</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -5720,7 +5723,7 @@
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B37">
         <f>Principal!$E$27</f>
-        <v>130</v>
+        <v>180</v>
       </c>
       <c r="C37">
         <v>0</v>

</xml_diff>

<commit_message>
Ready for final exam
Everything ready for the final, so we are in THE FINAL COUNTDOWN
</commit_message>
<xml_diff>
--- a/Documentation/Fuzzy/Fuzzy Table.xlsx
+++ b/Documentation/Fuzzy/Fuzzy Table.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="43">
   <si>
     <t>2 Entradas:</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>asi que lo offseteo con +50 para fuzzy</t>
+  </si>
+  <si>
+    <t>Expandidos en decimal</t>
   </si>
 </sst>
 </file>
@@ -454,10 +457,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>40</c:v>
@@ -536,10 +539,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>70</c:v>
@@ -618,10 +621,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>70</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>80</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>100</c:v>
@@ -700,10 +703,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>110</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>120</c:v>
@@ -782,10 +785,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>120</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>130</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>145</c:v>
@@ -864,13 +867,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>145</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>155</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>179</c:v>
+                  <c:v>178</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>180</c:v>
@@ -909,11 +912,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="223154656"/>
-        <c:axId val="223155216"/>
+        <c:axId val="236416224"/>
+        <c:axId val="236416784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="223154656"/>
+        <c:axId val="236416224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -971,13 +974,13 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223155216"/>
+        <c:crossAx val="236416784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="223155216"/>
+        <c:axId val="236416784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -1036,7 +1039,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223154656"/>
+        <c:crossAx val="236416224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -1213,7 +1216,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>10</c:v>
@@ -1292,7 +1295,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>20</c:v>
@@ -1371,10 +1374,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>45</c:v>
@@ -1453,10 +1456,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>45</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>75</c:v>
@@ -1535,10 +1538,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>75</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>85</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>99</c:v>
@@ -1580,11 +1583,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="286062016"/>
-        <c:axId val="286062576"/>
+        <c:axId val="236421824"/>
+        <c:axId val="236422384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="286062016"/>
+        <c:axId val="236421824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="110"/>
@@ -1642,13 +1645,13 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="286062576"/>
+        <c:crossAx val="236422384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="286062576"/>
+        <c:axId val="236422384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -1707,7 +1710,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="286062016"/>
+        <c:crossAx val="236421824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -1852,10 +1855,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>40</c:v>
@@ -1926,10 +1929,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>70</c:v>
@@ -2008,10 +2011,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>70</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>80</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>100</c:v>
@@ -2090,10 +2093,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>110</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>120</c:v>
@@ -2172,10 +2175,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>120</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>130</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>145</c:v>
@@ -2254,13 +2257,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>145</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>155</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>179</c:v>
+                  <c:v>178</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>180</c:v>
@@ -2299,11 +2302,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="286068176"/>
-        <c:axId val="286068736"/>
+        <c:axId val="308233024"/>
+        <c:axId val="308233584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="286068176"/>
+        <c:axId val="308233024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2360,12 +2363,12 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="286068736"/>
+        <c:crossAx val="308233584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="286068736"/>
+        <c:axId val="308233584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2422,7 +2425,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="286068176"/>
+        <c:crossAx val="308233024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4528,10 +4531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N51"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4822,10 +4825,10 @@
         <v>8</v>
       </c>
       <c r="B22">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C22">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D22">
         <v>40</v>
@@ -4839,10 +4842,10 @@
         <v>9</v>
       </c>
       <c r="B23">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C23">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D23">
         <v>70</v>
@@ -4856,10 +4859,10 @@
         <v>10</v>
       </c>
       <c r="B24">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C24">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D24">
         <v>100</v>
@@ -4873,10 +4876,10 @@
         <v>11</v>
       </c>
       <c r="B25">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C25">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D25">
         <v>120</v>
@@ -4890,10 +4893,10 @@
         <v>12</v>
       </c>
       <c r="B26">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C26">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D26">
         <v>145</v>
@@ -4907,13 +4910,13 @@
         <v>13</v>
       </c>
       <c r="B27">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C27">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D27">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E27">
         <v>180</v>
@@ -4952,14 +4955,14 @@
         <v>1</v>
       </c>
       <c r="D32">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E32">
         <v>10</v>
       </c>
       <c r="N32" s="1"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -4967,7 +4970,7 @@
         <v>5</v>
       </c>
       <c r="C33">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D33">
         <v>20</v>
@@ -4976,15 +4979,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>16</v>
       </c>
       <c r="B34">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C34">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D34">
         <v>45</v>
@@ -4993,15 +4996,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>17</v>
       </c>
       <c r="B35">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C35">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D35">
         <v>75</v>
@@ -5010,15 +5013,15 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>18</v>
       </c>
       <c r="B36">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C36">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D36">
         <v>99</v>
@@ -5027,7 +5030,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -5037,18 +5040,21 @@
       <c r="G38" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>8</v>
       </c>
       <c r="B40" t="str">
         <f>DEC2HEX( (255*B22/190))</f>
-        <v>D</v>
+        <v>0</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" ref="C40:E40" si="0">DEC2HEX( (255*C22/190))</f>
-        <v>E</v>
+        <v>4</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
@@ -5060,11 +5066,11 @@
       </c>
       <c r="G40" t="str">
         <f>B40</f>
-        <v>D</v>
+        <v>0</v>
       </c>
       <c r="H40" t="str">
         <f>DEC2HEX((255+(((HEX2DEC(C40))-(HEX2DEC(B40)))/2))/((HEX2DEC(C40))-(HEX2DEC(B40))))</f>
-        <v>FF</v>
+        <v>40</v>
       </c>
       <c r="I40" t="str">
         <f>D40</f>
@@ -5074,193 +5080,289 @@
         <f>DEC2HEX((255+(((HEX2DEC(E40))-(HEX2DEC(D40)))/2))/((HEX2DEC(E40))-(HEX2DEC(D40))))</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L40">
+        <f>(255*B22/190)</f>
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <f t="shared" ref="M40:O40" si="1">(255*C22/190)</f>
+        <v>4.0263157894736841</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="1"/>
+        <v>53.684210526315788</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="1"/>
+        <v>67.10526315789474</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>9</v>
       </c>
       <c r="B41" t="str">
-        <f t="shared" ref="B41:E45" si="1">DEC2HEX( (255*B23/190))</f>
-        <v>35</v>
+        <f t="shared" ref="B41:E45" si="2">DEC2HEX( (255*B23/190))</f>
+        <v>2E</v>
       </c>
       <c r="C41" t="str">
-        <f t="shared" si="1"/>
-        <v>43</v>
+        <f t="shared" si="2"/>
+        <v>3C</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5D</v>
       </c>
       <c r="E41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6B</v>
       </c>
       <c r="G41" t="str">
-        <f t="shared" ref="G41:G51" si="2">B41</f>
-        <v>35</v>
+        <f t="shared" ref="G41:G51" si="3">B41</f>
+        <v>2E</v>
       </c>
       <c r="H41" t="str">
-        <f t="shared" ref="H41:H51" si="3">DEC2HEX((255+(((HEX2DEC(C41))-(HEX2DEC(B41)))/2))/((HEX2DEC(C41))-(HEX2DEC(B41))))</f>
+        <f t="shared" ref="H41:H51" si="4">DEC2HEX((255+(((HEX2DEC(C41))-(HEX2DEC(B41)))/2))/((HEX2DEC(C41))-(HEX2DEC(B41))))</f>
         <v>12</v>
       </c>
       <c r="I41" t="str">
-        <f t="shared" ref="I41:I51" si="4">D41</f>
+        <f t="shared" ref="I41:I51" si="5">D41</f>
         <v>5D</v>
       </c>
       <c r="J41" t="str">
-        <f t="shared" ref="J41:J51" si="5">DEC2HEX((255+(((HEX2DEC(E41))-(HEX2DEC(D41)))/2))/((HEX2DEC(E41))-(HEX2DEC(D41))))</f>
+        <f t="shared" ref="J41:J51" si="6">DEC2HEX((255+(((HEX2DEC(E41))-(HEX2DEC(D41)))/2))/((HEX2DEC(E41))-(HEX2DEC(D41))))</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L41">
+        <f t="shared" ref="L41:L45" si="7">(255*B23/190)</f>
+        <v>46.973684210526315</v>
+      </c>
+      <c r="M41">
+        <f t="shared" ref="M41:M45" si="8">(255*C23/190)</f>
+        <v>60.39473684210526</v>
+      </c>
+      <c r="N41">
+        <f t="shared" ref="N41:N45" si="9">(255*D23/190)</f>
+        <v>93.94736842105263</v>
+      </c>
+      <c r="O41">
+        <f t="shared" ref="O41:O45" si="10">(255*E23/190)</f>
+        <v>107.36842105263158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>10</v>
       </c>
       <c r="B42" t="str">
-        <f t="shared" si="1"/>
-        <v>5D</v>
+        <f t="shared" si="2"/>
+        <v>57</v>
       </c>
       <c r="C42" t="str">
-        <f t="shared" si="1"/>
-        <v>6B</v>
+        <f t="shared" si="2"/>
+        <v>64</v>
       </c>
       <c r="D42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>86</v>
       </c>
       <c r="E42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>93</v>
       </c>
       <c r="G42" t="str">
-        <f t="shared" si="2"/>
-        <v>5D</v>
+        <f t="shared" si="3"/>
+        <v>57</v>
       </c>
       <c r="H42" t="str">
-        <f t="shared" si="3"/>
-        <v>12</v>
+        <f t="shared" si="4"/>
+        <v>14</v>
       </c>
       <c r="I42" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>86</v>
       </c>
       <c r="J42" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L42">
+        <f t="shared" si="7"/>
+        <v>87.236842105263165</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="8"/>
+        <v>100.65789473684211</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="9"/>
+        <v>134.21052631578948</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="10"/>
+        <v>147.63157894736841</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>11</v>
       </c>
       <c r="B43" t="str">
-        <f t="shared" si="1"/>
-        <v>86</v>
+        <f t="shared" si="2"/>
+        <v>7F</v>
       </c>
       <c r="C43" t="str">
-        <f t="shared" si="1"/>
-        <v>93</v>
+        <f t="shared" si="2"/>
+        <v>8C</v>
       </c>
       <c r="D43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A1</v>
       </c>
       <c r="E43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>AE</v>
       </c>
       <c r="G43" t="str">
-        <f t="shared" si="2"/>
-        <v>86</v>
+        <f t="shared" si="3"/>
+        <v>7F</v>
       </c>
       <c r="H43" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="I43" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>A1</v>
       </c>
       <c r="J43" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L43">
+        <f t="shared" si="7"/>
+        <v>127.5</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="8"/>
+        <v>140.92105263157896</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="9"/>
+        <v>161.05263157894737</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="10"/>
+        <v>174.47368421052633</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>12</v>
       </c>
       <c r="B44" t="str">
-        <f t="shared" si="1"/>
-        <v>A1</v>
+        <f t="shared" si="2"/>
+        <v>9A</v>
       </c>
       <c r="C44" t="str">
-        <f t="shared" si="1"/>
-        <v>AE</v>
+        <f t="shared" si="2"/>
+        <v>A7</v>
       </c>
       <c r="D44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>C2</v>
       </c>
       <c r="E44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>D0</v>
       </c>
       <c r="G44" t="str">
-        <f t="shared" si="2"/>
-        <v>A1</v>
+        <f t="shared" si="3"/>
+        <v>9A</v>
       </c>
       <c r="H44" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="I44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>C2</v>
       </c>
       <c r="J44" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L44">
+        <f t="shared" si="7"/>
+        <v>154.34210526315789</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="8"/>
+        <v>167.76315789473685</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="9"/>
+        <v>194.60526315789474</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="10"/>
+        <v>208.02631578947367</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>13</v>
       </c>
       <c r="B45" t="str">
-        <f t="shared" si="1"/>
-        <v>C2</v>
+        <f t="shared" si="2"/>
+        <v>B5</v>
       </c>
       <c r="C45" t="str">
-        <f t="shared" si="1"/>
-        <v>D0</v>
+        <f t="shared" si="2"/>
+        <v>C9</v>
       </c>
       <c r="D45" t="str">
-        <f t="shared" si="1"/>
-        <v>F0</v>
+        <f t="shared" si="2"/>
+        <v>EE</v>
       </c>
       <c r="E45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>F1</v>
       </c>
       <c r="G45" t="str">
-        <f t="shared" si="2"/>
-        <v>C2</v>
+        <f t="shared" si="3"/>
+        <v>B5</v>
       </c>
       <c r="H45" t="str">
-        <f t="shared" si="3"/>
-        <v>12</v>
+        <f t="shared" si="4"/>
+        <v>D</v>
       </c>
       <c r="I45" t="str">
-        <f t="shared" si="4"/>
-        <v>F0</v>
+        <f t="shared" si="5"/>
+        <v>EE</v>
       </c>
       <c r="J45" t="str">
-        <f t="shared" si="5"/>
-        <v>FF</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+        <f t="shared" si="6"/>
+        <v>55</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="7"/>
+        <v>181.18421052631578</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="8"/>
+        <v>201.31578947368422</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="9"/>
+        <v>238.89473684210526</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="10"/>
+        <v>241.57894736842104</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -5269,180 +5371,260 @@
         <v>0</v>
       </c>
       <c r="C47" t="str">
-        <f t="shared" ref="C47:E47" si="6">DEC2HEX( (255*C32/100))</f>
+        <f t="shared" ref="C47:E47" si="11">DEC2HEX( (255*C32/100))</f>
         <v>2</v>
       </c>
       <c r="D47" t="str">
+        <f t="shared" si="11"/>
+        <v>F</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="11"/>
+        <v>19</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H47" t="str">
+        <f t="shared" si="4"/>
+        <v>80</v>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" si="5"/>
+        <v>F</v>
+      </c>
+      <c r="J47" t="str">
         <f t="shared" si="6"/>
+        <v>1A</v>
+      </c>
+      <c r="L47">
+        <f xml:space="preserve"> (255*B32/100)</f>
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <f t="shared" ref="M47:O47" si="12" xml:space="preserve"> (255*C32/100)</f>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="12"/>
+        <v>15.3</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="12"/>
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>15</v>
+      </c>
+      <c r="B48" t="str">
+        <f t="shared" ref="B48:E48" si="13">DEC2HEX( (255*B33/100))</f>
         <v>C</v>
       </c>
-      <c r="E47" t="str">
+      <c r="C48" t="str">
+        <f t="shared" si="13"/>
+        <v>14</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="13"/>
+        <v>33</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="13"/>
+        <v>3F</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="3"/>
+        <v>C</v>
+      </c>
+      <c r="H48" t="str">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" si="5"/>
+        <v>33</v>
+      </c>
+      <c r="J48" t="str">
         <f t="shared" si="6"/>
-        <v>19</v>
-      </c>
-      <c r="G47" t="str">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H47" t="str">
+        <v>15</v>
+      </c>
+      <c r="L48">
+        <f t="shared" ref="L48:L51" si="14" xml:space="preserve"> (255*B33/100)</f>
+        <v>12.75</v>
+      </c>
+      <c r="M48">
+        <f t="shared" ref="M48:M51" si="15" xml:space="preserve"> (255*C33/100)</f>
+        <v>20.399999999999999</v>
+      </c>
+      <c r="N48">
+        <f t="shared" ref="N48:N51" si="16" xml:space="preserve"> (255*D33/100)</f>
+        <v>51</v>
+      </c>
+      <c r="O48">
+        <f t="shared" ref="O48:O51" si="17" xml:space="preserve"> (255*E33/100)</f>
+        <v>63.75</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" ref="B49:E49" si="18">DEC2HEX( (255*B34/100))</f>
+        <v>2D</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="18"/>
+        <v>3A</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="18"/>
+        <v>72</v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="18"/>
+        <v>8C</v>
+      </c>
+      <c r="G49" t="str">
         <f t="shared" si="3"/>
-        <v>80</v>
-      </c>
-      <c r="I47" t="str">
+        <v>2D</v>
+      </c>
+      <c r="H49" t="str">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" si="5"/>
+        <v>72</v>
+      </c>
+      <c r="J49" t="str">
+        <f t="shared" si="6"/>
+        <v>A</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="14"/>
+        <v>45.9</v>
+      </c>
+      <c r="M49">
+        <f t="shared" si="15"/>
+        <v>58.65</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="16"/>
+        <v>114.75</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="17"/>
+        <v>140.25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>17</v>
+      </c>
+      <c r="B50" t="str">
+        <f t="shared" ref="B50:E50" si="19">DEC2HEX( (255*B35/100))</f>
+        <v>6B</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="19"/>
+        <v>84</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="19"/>
+        <v>BF</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="19"/>
+        <v>D8</v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="3"/>
+        <v>6B</v>
+      </c>
+      <c r="H50" t="str">
+        <f t="shared" si="4"/>
+        <v>A</v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="5"/>
+        <v>BF</v>
+      </c>
+      <c r="J50" t="str">
+        <f t="shared" si="6"/>
+        <v>A</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="14"/>
+        <v>107.1</v>
+      </c>
+      <c r="M50">
+        <f t="shared" si="15"/>
+        <v>132.6</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="16"/>
+        <v>191.25</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="17"/>
+        <v>216.75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>18</v>
+      </c>
+      <c r="B51" t="str">
+        <f t="shared" ref="B51:E51" si="20">DEC2HEX( (255*B36/100))</f>
+        <v>B7</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="20"/>
+        <v>CC</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="20"/>
+        <v>FC</v>
+      </c>
+      <c r="E51" t="str">
+        <f t="shared" si="20"/>
+        <v>FF</v>
+      </c>
+      <c r="G51" t="str">
+        <f t="shared" si="3"/>
+        <v>B7</v>
+      </c>
+      <c r="H51" t="str">
         <f t="shared" si="4"/>
         <v>C</v>
       </c>
-      <c r="J47" t="str">
+      <c r="I51" t="str">
         <f t="shared" si="5"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>15</v>
-      </c>
-      <c r="B48" t="str">
-        <f t="shared" ref="B48:E48" si="7">DEC2HEX( (255*B33/100))</f>
-        <v>C</v>
-      </c>
-      <c r="C48" t="str">
-        <f t="shared" si="7"/>
-        <v>19</v>
-      </c>
-      <c r="D48" t="str">
-        <f t="shared" si="7"/>
-        <v>33</v>
-      </c>
-      <c r="E48" t="str">
-        <f t="shared" si="7"/>
-        <v>3F</v>
-      </c>
-      <c r="G48" t="str">
-        <f t="shared" si="2"/>
-        <v>C</v>
-      </c>
-      <c r="H48" t="str">
-        <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="I48" t="str">
-        <f t="shared" si="4"/>
-        <v>33</v>
-      </c>
-      <c r="J48" t="str">
-        <f t="shared" si="5"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>16</v>
-      </c>
-      <c r="B49" t="str">
-        <f t="shared" ref="B49:E49" si="8">DEC2HEX( (255*B34/100))</f>
-        <v>33</v>
-      </c>
-      <c r="C49" t="str">
-        <f t="shared" si="8"/>
-        <v>3F</v>
-      </c>
-      <c r="D49" t="str">
-        <f t="shared" si="8"/>
-        <v>72</v>
-      </c>
-      <c r="E49" t="str">
-        <f t="shared" si="8"/>
-        <v>8C</v>
-      </c>
-      <c r="G49" t="str">
-        <f t="shared" si="2"/>
-        <v>33</v>
-      </c>
-      <c r="H49" t="str">
-        <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="I49" t="str">
-        <f t="shared" si="4"/>
-        <v>72</v>
-      </c>
-      <c r="J49" t="str">
-        <f t="shared" si="5"/>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>17</v>
-      </c>
-      <c r="B50" t="str">
-        <f t="shared" ref="B50:E50" si="9">DEC2HEX( (255*B35/100))</f>
-        <v>72</v>
-      </c>
-      <c r="C50" t="str">
-        <f t="shared" si="9"/>
-        <v>8C</v>
-      </c>
-      <c r="D50" t="str">
-        <f t="shared" si="9"/>
-        <v>BF</v>
-      </c>
-      <c r="E50" t="str">
-        <f t="shared" si="9"/>
-        <v>D8</v>
-      </c>
-      <c r="G50" t="str">
-        <f t="shared" si="2"/>
-        <v>72</v>
-      </c>
-      <c r="H50" t="str">
-        <f t="shared" si="3"/>
-        <v>A</v>
-      </c>
-      <c r="I50" t="str">
-        <f t="shared" si="4"/>
-        <v>BF</v>
-      </c>
-      <c r="J50" t="str">
-        <f t="shared" si="5"/>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>18</v>
-      </c>
-      <c r="B51" t="str">
-        <f t="shared" ref="B51:E51" si="10">DEC2HEX( (255*B36/100))</f>
-        <v>BF</v>
-      </c>
-      <c r="C51" t="str">
-        <f t="shared" si="10"/>
-        <v>D8</v>
-      </c>
-      <c r="D51" t="str">
-        <f t="shared" si="10"/>
         <v>FC</v>
       </c>
-      <c r="E51" t="str">
-        <f t="shared" si="10"/>
-        <v>FF</v>
-      </c>
-      <c r="G51" t="str">
-        <f t="shared" si="2"/>
-        <v>BF</v>
-      </c>
-      <c r="H51" t="str">
-        <f t="shared" si="3"/>
-        <v>A</v>
-      </c>
-      <c r="I51" t="str">
-        <f t="shared" si="4"/>
-        <v>FC</v>
-      </c>
       <c r="J51" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>55</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="14"/>
+        <v>183.6</v>
+      </c>
+      <c r="M51">
+        <f t="shared" si="15"/>
+        <v>204</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="16"/>
+        <v>252.45</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="17"/>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -5479,7 +5661,7 @@
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4">
         <f>Principal!$B$22</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -5488,7 +5670,7 @@
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5">
         <f>Principal!$C$22</f>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -5526,7 +5708,7 @@
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10">
         <f>Principal!$B$23</f>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -5535,7 +5717,7 @@
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11">
         <f>Principal!$C$23</f>
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -5573,7 +5755,7 @@
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16">
         <f>Principal!$B$24</f>
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -5582,7 +5764,7 @@
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B17">
         <f>Principal!$C$24</f>
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -5620,7 +5802,7 @@
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B22">
         <f>Principal!$B$25</f>
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -5629,7 +5811,7 @@
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B23">
         <f>Principal!$C$25</f>
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -5667,7 +5849,7 @@
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B28">
         <f>Principal!$B$26</f>
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -5676,7 +5858,7 @@
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B29">
         <f>Principal!$C$26</f>
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -5714,7 +5896,7 @@
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B34">
         <f>Principal!$B$27</f>
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -5723,7 +5905,7 @@
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B35">
         <f>Principal!$C$27</f>
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -5732,7 +5914,7 @@
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B36">
         <f>Principal!$D$27</f>
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C36">
         <v>1</v>

</xml_diff>